<commit_message>
Addition of new measurements as of 21/04/2022.
</commit_message>
<xml_diff>
--- a/band-pass-filter.xlsx
+++ b/band-pass-filter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niccolozanotti/Library/Application Support/JetBrains/DataSpell2021.3/projects/Lab II/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5A7AB5-648C-C643-859D-5EEE036B86C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F060EE-5249-9249-A57D-97102242FA86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="3240" windowWidth="27640" windowHeight="16940" xr2:uid="{4A92E359-DC56-554D-B3DE-C1EC25D98A90}"/>
+    <workbookView xWindow="920" yWindow="2700" windowWidth="27640" windowHeight="16940" xr2:uid="{4A92E359-DC56-554D-B3DE-C1EC25D98A90}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Nominal value</t>
   </si>
@@ -94,6 +94,21 @@
   <si>
     <t>Quality factor(Q)</t>
   </si>
+  <si>
+    <t>L(mH)</t>
+  </si>
+  <si>
+    <t>C(nF)</t>
+  </si>
+  <si>
+    <t>costante a 1.460/61</t>
+  </si>
+  <si>
+    <t>L MEDIO(H)</t>
+  </si>
+  <si>
+    <t>(DA VALUTARE)</t>
+  </si>
 </sst>
 </file>
 
@@ -104,9 +119,16 @@
     <numFmt numFmtId="165" formatCode="0.0000E+00"/>
     <numFmt numFmtId="166" formatCode="0.0E+00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -139,6 +161,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -160,39 +189,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -270,10 +308,6 @@
     <xdr:clientData/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -573,17 +607,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{874FE816-04C9-114E-B24F-8139CF21F075}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="177" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5" style="1" customWidth="1"/>
     <col min="2" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" style="1"/>
     <col min="9" max="9" width="23.33203125" style="1" customWidth="1"/>
@@ -662,36 +696,37 @@
         <v>1</v>
       </c>
       <c r="B3" s="9">
-        <v>998.5</v>
+        <v>996.7</v>
       </c>
       <c r="C3" s="10">
-        <v>4.7669999999999997E-2</v>
+        <f>AVERAGE(B11:B30)*10^(-3)</f>
+        <v>4.7412999999999983E-2</v>
       </c>
       <c r="D3" s="10">
-        <v>1.4889999999999999E-9</v>
+        <v>1.4599999999999999E-9</v>
       </c>
       <c r="E3" s="6">
         <v>50</v>
       </c>
       <c r="F3" s="11">
-        <v>125.77</v>
+        <v>125.82</v>
       </c>
       <c r="G3" s="6">
         <f>B3+E3+F3</f>
-        <v>1174.27</v>
+        <v>1172.52</v>
       </c>
       <c r="H3" s="6"/>
       <c r="I3" s="10">
         <f>1/SQRT(C3*D3)</f>
-        <v>118694.35783728464</v>
+        <v>120191.80416237816</v>
       </c>
       <c r="J3" s="10">
         <f>I3/(2*PI())</f>
-        <v>18890.793766922099</v>
+        <v>19129.119751575527</v>
       </c>
       <c r="K3" s="10">
         <f>I3*C3/G3</f>
-        <v>4.8184489411322424</v>
+        <v>4.8601763814270402</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -700,30 +735,165 @@
       </c>
       <c r="B4" s="7">
         <f>450/1000000*B3+100/1000000*10000</f>
-        <v>1.449325</v>
+        <v>1.448515</v>
       </c>
       <c r="C4" s="8">
         <f>1/100*C3</f>
-        <v>4.7669999999999999E-4</v>
+        <v>4.7412999999999985E-4</v>
       </c>
       <c r="D4" s="8">
         <f>1/100*D3</f>
-        <v>1.489E-11</v>
+        <v>1.46E-11</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="8">
         <f>450/1000000*F3+100/1000000*1000</f>
-        <v>0.1565965</v>
+        <v>0.15661900000000001</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5">
         <f>SQRT((1/2*(C3*D3)^(-3/2)*D3*C4)^2+(1/2*(C3*D3)^(-3/2)*C3*D4)^2)</f>
-        <v>839.29585315326722</v>
+        <v>849.884397662629</v>
       </c>
       <c r="J4" s="5">
         <f xml:space="preserve"> I4/(2*PI())</f>
-        <v>133.57808374587199</v>
+        <v>135.26330294468548</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C5" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F6" s="11"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F8" s="14"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <f>AVERAGE(B11:B30)*10^(-3)</f>
+        <v>4.7412999999999983E-2</v>
+      </c>
+      <c r="B11" s="1">
+        <v>47.45</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>47.43</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1.4690000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>47.42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>47.42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>47.42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>47.42</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>47.41</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>47.41</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>47.41</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <v>47.41</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>47.41</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>47.41</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>47.41</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>47.41</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>47.41</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>47.41</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="13">
+        <v>47.4</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="13">
+        <v>47.4</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="13">
+        <v>47.4</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="13">
+        <v>47.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>